<commit_message>
Added get mac address from name when on macos
</commit_message>
<xml_diff>
--- a/makeblock_robots.xlsx
+++ b/makeblock_robots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_data\projets\arduino\auriga_bluetooth_python_comm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{864BA38C-C31F-4E39-88E1-FFF8CB51B0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0490B40-D0CE-4E09-ACB0-1BE4E4C0D753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E573B4E6-D275-4F68-A8F6-FC60B9EDC9ED}"/>
   </bookViews>
@@ -1141,7 +1141,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="A1:D28"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,5 +1469,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>